<commit_message>
In  function is_rowwise, it makes no sense to check for numerical values if the frequency has been specified with a value greater than one. read_ts_xlsx now determines the sheetname for error messages correctly.
</commit_message>
<xml_diff>
--- a/pkg/tests/testthat/read_ts/xlsx/example13.xlsx
+++ b/pkg/tests/testthat/read_ts/xlsx/example13.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Output of the CEP 2017</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">(EUR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxx</t>
   </si>
   <si>
     <t xml:space="preserve">2011q2</t>
@@ -158,19 +161,19 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,8 +209,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>6</v>
@@ -218,7 +224,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>5</v>
@@ -229,17 +235,17 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>

</xml_diff>